<commit_message>
Highlighting és preview részt kéne megcsinálni
</commit_message>
<xml_diff>
--- a/Megnyirtások.xlsx
+++ b/Megnyirtások.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mszabo\Desktop\NotWork\BeGreatDev\JS\SandBox\VanillaJS Chesopenings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3DB9F2C-2A20-4EBE-B269-53533C72D1E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB573FB6-035A-48F7-9297-FC6B81D74D8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
   <si>
     <t>Queen's gambit</t>
   </si>
@@ -87,21 +87,12 @@
     <t>19. lépés</t>
   </si>
   <si>
-    <t>d4</t>
-  </si>
-  <si>
-    <t>d5</t>
-  </si>
-  <si>
     <t>Fehér</t>
   </si>
   <si>
     <t>Fekete</t>
   </si>
   <si>
-    <t>c4</t>
-  </si>
-  <si>
     <t>Queen's gambit declined</t>
   </si>
   <si>
@@ -109,6 +100,42 @@
   </si>
   <si>
     <t>Leírás</t>
+  </si>
+  <si>
+    <t>d2-d4</t>
+  </si>
+  <si>
+    <t>d7-d5</t>
+  </si>
+  <si>
+    <t>c2-c4</t>
+  </si>
+  <si>
+    <t>d5-c4</t>
+  </si>
+  <si>
+    <t>g1-f3</t>
+  </si>
+  <si>
+    <t>g8-f6</t>
+  </si>
+  <si>
+    <t>e2-e3</t>
+  </si>
+  <si>
+    <t>e7-e6</t>
+  </si>
+  <si>
+    <t>f1-c4</t>
+  </si>
+  <si>
+    <t>c7-c5</t>
+  </si>
+  <si>
+    <t>0-0</t>
+  </si>
+  <si>
+    <t>a7-a6</t>
   </si>
 </sst>
 </file>
@@ -283,47 +310,57 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -606,10 +643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.35"/>
@@ -618,292 +655,357 @@
     <col min="2" max="2" width="8.88671875" style="1"/>
     <col min="3" max="3" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22" style="1" customWidth="1"/>
-    <col min="7" max="7" width="22.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.109375" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="1"/>
+    <col min="5" max="5" width="8.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="22" style="1" customWidth="1"/>
+    <col min="8" max="8" width="22.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="19.109375" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.4">
       <c r="A1" s="2"/>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="7" t="s">
+      <c r="C1" s="13"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="13"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="13"/>
+      <c r="J1" s="12"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" s="5"/>
+      <c r="B2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="8"/>
-      <c r="G1" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1" s="8"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="11"/>
-      <c r="B2" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="18" t="s">
+      <c r="D3" s="7"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="16"/>
+    </row>
+    <row r="4" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="4"/>
-    </row>
-    <row r="4" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="4"/>
-    </row>
-    <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="11" t="s">
+      <c r="C4" s="9"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="7"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="16"/>
+    </row>
+    <row r="5" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="4"/>
-    </row>
-    <row r="6" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="11" t="s">
+      <c r="B5" s="3"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="7"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="16"/>
+    </row>
+    <row r="6" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="4"/>
-    </row>
-    <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="11" t="s">
+      <c r="B6" s="3"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="7"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="16"/>
+    </row>
+    <row r="7" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="4"/>
-    </row>
-    <row r="8" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="11" t="s">
+      <c r="B7" s="3"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" s="7"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="16"/>
+    </row>
+    <row r="8" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="4"/>
-    </row>
-    <row r="9" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="11" t="s">
+      <c r="B8" s="3"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="7"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="16"/>
+    </row>
+    <row r="9" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="4"/>
-    </row>
-    <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="11" t="s">
+      <c r="B9" s="3"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="16"/>
+    </row>
+    <row r="10" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="4"/>
-    </row>
-    <row r="11" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="11" t="s">
+      <c r="B10" s="3"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="16"/>
+    </row>
+    <row r="11" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="4"/>
-    </row>
-    <row r="12" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="11" t="s">
+      <c r="B11" s="3"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="16"/>
+    </row>
+    <row r="12" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="4"/>
-    </row>
-    <row r="13" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="11" t="s">
+      <c r="B12" s="3"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="16"/>
+    </row>
+    <row r="13" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="4"/>
-    </row>
-    <row r="14" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="11" t="s">
+      <c r="B13" s="3"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="16"/>
+    </row>
+    <row r="14" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="9"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="4"/>
-    </row>
-    <row r="15" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="11" t="s">
+      <c r="B14" s="3"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="16"/>
+    </row>
+    <row r="15" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="4"/>
-    </row>
-    <row r="16" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="11" t="s">
+      <c r="B15" s="3"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="16"/>
+    </row>
+    <row r="16" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="9"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="4"/>
-    </row>
-    <row r="17" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="11" t="s">
+      <c r="B16" s="3"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="16"/>
+    </row>
+    <row r="17" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="9"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="4"/>
-    </row>
-    <row r="18" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="11" t="s">
+      <c r="B17" s="3"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="16"/>
+    </row>
+    <row r="18" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="9"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="4"/>
-    </row>
-    <row r="19" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="11" t="s">
+      <c r="B18" s="3"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="16"/>
+    </row>
+    <row r="19" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="9"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="4"/>
-    </row>
-    <row r="20" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="11" t="s">
+      <c r="B19" s="3"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="16"/>
+    </row>
+    <row r="20" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="9"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="4"/>
-    </row>
-    <row r="21" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="11" t="s">
+      <c r="B20" s="3"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="16"/>
+    </row>
+    <row r="21" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="16"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="E1:F1"/>
     <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:J1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>